<commit_message>
1. Refactored SolarFinancialModel to consolidate all scenario summaries into a single summary sheet.
2. Added logic for energy export option in the input file, allowing conditional gains from TNB buyback.

3. Updated GITA tax savings calculation to correctly account for base investment cost.
</commit_message>
<xml_diff>
--- a/solar_financial_model_inputs.xlsx
+++ b/solar_financial_model_inputs.xlsx
@@ -8,21 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dialogasia.sharepoint.com/sites/oe-departmental/Green COE/2. Decarbonisation/1. Green Energy/1. Solar Power/1. Evaluations/model-generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="11_3043975BDCA17382A1F957965959A679F41E36D5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BE469E6-8A7F-4F43-A758-E753709623E9}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="11_3043975BDCA17382A1F957965959A679F41E36D5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9856CE20-0B55-4C56-A42F-CC55BE7E7376}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input Details" sheetId="1" r:id="rId1"/>
     <sheet name="Scenarios" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Capacity (kWp)</t>
   </si>
@@ -100,6 +99,9 @@
   </si>
   <si>
     <t>increase_then_reduce</t>
+  </si>
+  <si>
+    <t>Energy Export Allowed</t>
   </si>
 </sst>
 </file>
@@ -128,7 +130,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -151,13 +153,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -462,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,7 +504,7 @@
     <col min="16" max="16" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -537,8 +553,11 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>88</v>
       </c>
@@ -549,7 +568,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E2">
         <v>0.29799999999999999</v>
@@ -587,8 +606,11 @@
       <c r="P2">
         <v>2</v>
       </c>
+      <c r="Q2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>18.27</v>
       </c>
@@ -599,7 +621,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E3">
         <v>0.29799999999999999</v>
@@ -637,8 +659,11 @@
       <c r="P3">
         <v>2</v>
       </c>
+      <c r="Q3" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>65.540000000000006</v>
       </c>
@@ -649,7 +674,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E4">
         <v>0.29799999999999999</v>
@@ -686,6 +711,9 @@
       </c>
       <c r="P4">
         <v>2</v>
+      </c>
+      <c r="Q4" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -700,7 +728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -803,6 +831,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f3818e54-6791-4167-8bdf-6fd6e2741687" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a6b398a-4bb9-414e-8c3f-3e6482c1e9ed">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B189C0425820694BB39C66E1D63C456C" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="de6efd98d7fcb2a854f25e31bf44d29a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7a6b398a-4bb9-414e-8c3f-3e6482c1e9ed" xmlns:ns3="f3818e54-6791-4167-8bdf-6fd6e2741687" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2223ec9ff43e0fc63d8de49e750e241b" ns2:_="" ns3:_="">
     <xsd:import namespace="7a6b398a-4bb9-414e-8c3f-3e6482c1e9ed"/>
@@ -1037,7 +1076,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1046,25 +1085,40 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f3818e54-6791-4167-8bdf-6fd6e2741687" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a6b398a-4bb9-414e-8c3f-3e6482c1e9ed">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED4CCDDE-A149-4E6D-BF99-223B1A0F8FB9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92AC2047-80D6-4D41-B5C9-9B9A587040B8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f3818e54-6791-4167-8bdf-6fd6e2741687"/>
+    <ds:schemaRef ds:uri="7a6b398a-4bb9-414e-8c3f-3e6482c1e9ed"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83312BAC-EDFE-492F-A17B-F381A99382C9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED4CCDDE-A149-4E6D-BF99-223B1A0F8FB9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7a6b398a-4bb9-414e-8c3f-3e6482c1e9ed"/>
+    <ds:schemaRef ds:uri="f3818e54-6791-4167-8bdf-6fd6e2741687"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92AC2047-80D6-4D41-B5C9-9B9A587040B8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83312BAC-EDFE-492F-A17B-F381A99382C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>